<commit_message>
Fixes to make envelope poptimsatoim worl
</commit_message>
<xml_diff>
--- a/11-Parameters/Dummy4Tests.xlsx
+++ b/11-Parameters/Dummy4Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6741C8BE-5F27-2B4E-BCB9-208C5B5EEDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EEE0E-69A1-9841-8A5C-3BB8F2DCA09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11740" yWindow="640" windowWidth="18500" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -90,6 +90,48 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SourceMode</t>
+  </si>
+  <si>
+    <t>Gaussian kinetic energy</t>
+  </si>
+  <si>
+    <t>SigmaX</t>
+  </si>
+  <si>
+    <t>Gaussian width, x</t>
+  </si>
+  <si>
+    <t>SigmaY</t>
+  </si>
+  <si>
+    <t>Gaussian width, y</t>
+  </si>
+  <si>
+    <t>MeanEnergy</t>
+  </si>
+  <si>
+    <t>Mean of guassian kinetic energy</t>
+  </si>
+  <si>
+    <t>SigmaEnergy</t>
+  </si>
+  <si>
+    <t>Sigma of guassian kinetic energy</t>
+  </si>
+  <si>
+    <t>MinCTheta</t>
+  </si>
+  <si>
+    <t>Minimum theta for flat cos theta</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
   </si>
 </sst>
 </file>
@@ -204,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -214,6 +256,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,9 +277,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -272,7 +317,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -378,7 +423,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -520,7 +565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,6 +687,158 @@
       </c>
       <c r="H4" s="3"/>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8">
+        <v>15</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.998</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixes to test scripts; all good
</commit_message>
<xml_diff>
--- a/11-Parameters/Dummy4Tests.xlsx
+++ b/11-Parameters/Dummy4Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EEE0E-69A1-9841-8A5C-3BB8F2DCA09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7A7AD4-5ABA-054B-91EF-2FF831A69F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11740" yWindow="640" windowWidth="18500" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Kinetic energy</t>
   </si>
   <si>
-    <t>LhARA</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Gaussian</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -634,14 +634,14 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -674,16 +674,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="3">
         <v>0.75</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -692,23 +692,23 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -716,25 +716,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -742,25 +742,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="8">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -768,16 +768,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="8">
         <v>15</v>
@@ -786,7 +786,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -794,16 +794,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="8">
         <v>0.3</v>
@@ -812,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -820,23 +820,23 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="9">
         <v>0.998</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>